<commit_message>
Add interactive slider to production performance chart
Implement frontend logic to dynamically filter chart data based on user-selected number of recent records using a range slider.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ab82b662-954a-45ad-9e37-a64a43e3529b
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 6cec81d2-77e4-4f52-8bfb-4958fe08ac97
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d7b551d1-b37d-40c2-8d39-61fe8a04a1c4/ab82b662-954a-45ad-9e37-a64a43e3529b/ZT1Iu2n
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Jumbo.xlsx
+++ b/Jumbo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://storaenso-my.sharepoint.com/personal/dariusz_buchalski_storaenso_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{2C740303-9498-4E1B-B999-D732A592522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F15B4F8E-0C9A-496F-8EF4-36EE939F2186}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{2C740303-9498-4E1B-B999-D732A592522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CF4CF80-B2B3-4F3C-85B9-6E277A944BB0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE0CCD2D-10B9-4F52-863F-7EF4C64C1846}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_3" localSheetId="0" hidden="1">Arkusz1!$A$1:$J$73</definedName>
+    <definedName name="ExternalData_3" localSheetId="0" hidden="1">Arkusz1!$A$1:$J$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="27">
   <si>
     <t>Segment</t>
   </si>
@@ -117,12 +117,42 @@
   <si>
     <t>Narastający czas [wh]</t>
   </si>
+  <si>
+    <t>mtf_costcenter_number</t>
+  </si>
+  <si>
+    <t>mtf_report_date</t>
+  </si>
+  <si>
+    <t>Prod_m2</t>
+  </si>
+  <si>
+    <t>WorkMin</t>
+  </si>
+  <si>
+    <t>Speed_m2_wh</t>
+  </si>
+  <si>
+    <t>Cum_Prod_m2</t>
+  </si>
+  <si>
+    <t>Cum_WorkMin</t>
+  </si>
+  <si>
+    <t>Cum_Speed_m2_wh</t>
+  </si>
+  <si>
+    <t>techniczne</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,16 +161,31 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -148,20 +193,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -170,7 +257,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -214,8 +301,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}" name="Raport" displayName="Raport" ref="A1:J73" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:J73" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}" name="Raport" displayName="Raport" ref="A1:J93" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:J93" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J73">
     <sortCondition ref="D2:D73"/>
   </sortState>
@@ -223,10 +310,10 @@
     <tableColumn id="2" xr3:uid="{A434A7BD-B920-46DC-B679-B95F31C0C848}" uniqueName="2" name="Segment" queryTableFieldId="2" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{C0E9884D-F486-48B7-87A5-4F055B5CB66D}" uniqueName="3" name="Brygada" queryTableFieldId="3" dataDxfId="5"/>
     <tableColumn id="11" xr3:uid="{F9452BD7-48CB-4743-BE47-B2D814028231}" uniqueName="11" name="Maszyna" queryTableFieldId="14" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{41D9B31B-1C8D-4046-97C1-641A0512F4FF}" uniqueName="1" name="Dzień" queryTableFieldId="1" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{1BE80ADB-A0F6-4E35-9F75-8589EBAC253C}" uniqueName="4" name="Produkcja dzienna [m2 ]" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{8ADC085E-8895-4FE1-B278-28AC47A635AF}" uniqueName="5" name="Czas pracy [wh]" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{F0074E8F-F181-49E0-AA94-E5179D277904}" uniqueName="10" name="Prędkość dzienna [m2/wh]" queryTableFieldId="13" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{41D9B31B-1C8D-4046-97C1-641A0512F4FF}" uniqueName="1" name="Dzień" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{1BE80ADB-A0F6-4E35-9F75-8589EBAC253C}" uniqueName="4" name="Produkcja dzienna [m2 ]" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{8ADC085E-8895-4FE1-B278-28AC47A635AF}" uniqueName="5" name="Czas pracy [wh]" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{F0074E8F-F181-49E0-AA94-E5179D277904}" uniqueName="10" name="Prędkość dzienna [m2/wh]" queryTableFieldId="13" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{0851AB8C-C656-465B-A3A0-36796443A497}" uniqueName="6" name="Narastająca produkcja [m2]" queryTableFieldId="16"/>
     <tableColumn id="7" xr3:uid="{F2C67B8B-BAF4-4581-B1A3-A0321B5720DA}" uniqueName="7" name="Narastający czas [wh]" queryTableFieldId="17"/>
     <tableColumn id="8" xr3:uid="{F02E25EB-ABDC-4BEA-A110-810B00100C01}" uniqueName="8" name="Narastająca prędkość [m2/wh]" queryTableFieldId="18"/>
@@ -552,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309D4C89-61CE-4AA4-A671-398E4FB3D027}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:N18"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,10 +654,12 @@
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,12 +691,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -619,27 +708,33 @@
         <v>64763.524799999999</v>
       </c>
       <c r="F2">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="G2">
-        <v>9964</v>
+        <v>10502</v>
       </c>
       <c r="H2">
         <v>64763.524799999999</v>
       </c>
       <c r="I2">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="J2">
-        <v>9964</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10502</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -651,27 +746,33 @@
         <v>64763.524799999999</v>
       </c>
       <c r="F3">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="G3">
-        <v>9964</v>
+        <v>10502</v>
       </c>
       <c r="H3">
         <v>64763.524799999999</v>
       </c>
       <c r="I3">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="J3">
-        <v>9964</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10502</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -680,30 +781,36 @@
         <v>46028</v>
       </c>
       <c r="E4">
-        <v>4209.6291119999996</v>
+        <v>12926.057144</v>
       </c>
       <c r="F4">
-        <v>17.716666666666669</v>
+        <v>101.73333333333333</v>
       </c>
       <c r="G4">
-        <v>14257</v>
+        <v>7623</v>
       </c>
       <c r="H4">
-        <v>4209.6291119999996</v>
+        <v>165033.37570399998</v>
       </c>
       <c r="I4">
-        <v>17.716666666666669</v>
+        <v>921.7833333333333</v>
       </c>
       <c r="J4">
-        <v>14257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10742</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -712,25 +819,31 @@
         <v>46028</v>
       </c>
       <c r="E5">
-        <v>100376.62003200001</v>
+        <v>4209.6291119999996</v>
       </c>
       <c r="F5">
-        <v>506.6</v>
+        <v>17.716666666666669</v>
       </c>
       <c r="G5">
-        <v>11888</v>
+        <v>14257</v>
       </c>
       <c r="H5">
-        <v>165140.14483200002</v>
+        <v>4209.6291119999996</v>
       </c>
       <c r="I5">
-        <v>896.6</v>
+        <v>17.716666666666669</v>
       </c>
       <c r="J5">
-        <v>11051</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>14257</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -747,27 +860,33 @@
         <v>83240.933775999991</v>
       </c>
       <c r="F6">
-        <v>387.15000000000003</v>
+        <v>359.15000000000003</v>
       </c>
       <c r="G6">
-        <v>12901</v>
+        <v>13906</v>
       </c>
       <c r="H6">
-        <v>83240.933775999991</v>
+        <v>174977.08706399999</v>
       </c>
       <c r="I6">
-        <v>387.15000000000003</v>
+        <v>839.15000000000009</v>
       </c>
       <c r="J6">
-        <v>12901</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12511</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -776,30 +895,36 @@
         <v>46028</v>
       </c>
       <c r="E7">
-        <v>12926.057144</v>
+        <v>1515.1814400000001</v>
       </c>
       <c r="F7">
-        <v>101.73333333333333</v>
+        <v>92.85</v>
       </c>
       <c r="G7">
-        <v>7623</v>
+        <v>979</v>
       </c>
       <c r="H7">
-        <v>77689.581944000005</v>
+        <v>25546.592196999998</v>
       </c>
       <c r="I7">
-        <v>491.73333333333335</v>
+        <v>955.85</v>
       </c>
       <c r="J7">
-        <v>9479</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1604</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -808,30 +933,36 @@
         <v>46028</v>
       </c>
       <c r="E8">
-        <v>17630.616907</v>
+        <v>8107.5806700000003</v>
       </c>
       <c r="F8">
-        <v>462.28333333333325</v>
+        <v>358.26666666666665</v>
       </c>
       <c r="G8">
-        <v>2288</v>
+        <v>1358</v>
       </c>
       <c r="H8">
-        <v>17630.616907</v>
+        <v>8107.5806700000003</v>
       </c>
       <c r="I8">
-        <v>462.28333333333325</v>
+        <v>358.26666666666665</v>
       </c>
       <c r="J8">
-        <v>2288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1358</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -840,30 +971,36 @@
         <v>46028</v>
       </c>
       <c r="E9">
-        <v>27253.379016999999</v>
+        <v>17630.616907</v>
       </c>
       <c r="F9">
-        <v>933.4</v>
+        <v>447.28333333333325</v>
       </c>
       <c r="G9">
-        <v>1752</v>
+        <v>2365</v>
       </c>
       <c r="H9">
-        <v>27253.379016999999</v>
+        <v>24235.672627</v>
       </c>
       <c r="I9">
-        <v>933.4</v>
+        <v>630.44999999999993</v>
       </c>
       <c r="J9">
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2307</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -872,30 +1009,36 @@
         <v>46028</v>
       </c>
       <c r="E10">
-        <v>1515.1814400000001</v>
+        <v>100376.62003200001</v>
       </c>
       <c r="F10">
-        <v>92.85</v>
+        <v>478.6</v>
       </c>
       <c r="G10">
-        <v>979</v>
+        <v>12584</v>
       </c>
       <c r="H10">
-        <v>1515.1814400000001</v>
+        <v>165140.14483200002</v>
       </c>
       <c r="I10">
-        <v>92.85</v>
+        <v>848.6</v>
       </c>
       <c r="J10">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11676</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -904,30 +1047,36 @@
         <v>46028</v>
       </c>
       <c r="E11">
-        <v>8107.5806700000003</v>
+        <v>27253.379016999999</v>
       </c>
       <c r="F11">
-        <v>378.26666666666665</v>
+        <v>898.4</v>
       </c>
       <c r="G11">
-        <v>1286</v>
+        <v>1820</v>
       </c>
       <c r="H11">
-        <v>8107.5806700000003</v>
+        <v>47718.473889000001</v>
       </c>
       <c r="I11">
-        <v>378.26666666666665</v>
+        <v>1675.2833333333333</v>
       </c>
       <c r="J11">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1709</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -936,30 +1085,36 @@
         <v>46029</v>
       </c>
       <c r="E12">
-        <v>17270.273280000001</v>
+        <v>32175.423279999999</v>
       </c>
       <c r="F12">
-        <v>132.65</v>
+        <v>185.41666666666666</v>
       </c>
       <c r="G12">
-        <v>7812</v>
+        <v>10412</v>
       </c>
       <c r="H12">
-        <v>21479.902392</v>
+        <v>197208.79898399996</v>
       </c>
       <c r="I12">
-        <v>150.36666666666667</v>
+        <v>1107.2</v>
       </c>
       <c r="J12">
-        <v>8571</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10687</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -968,25 +1123,25 @@
         <v>46029</v>
       </c>
       <c r="E13">
-        <v>141181.84984799998</v>
+        <v>17270.273280000001</v>
       </c>
       <c r="F13">
-        <v>798.06666666666661</v>
+        <v>132.65</v>
       </c>
       <c r="G13">
-        <v>10614</v>
+        <v>7812</v>
       </c>
       <c r="H13">
-        <v>306321.99468</v>
+        <v>170495.99692799998</v>
       </c>
       <c r="I13">
-        <v>1694.6666666666665</v>
+        <v>993.36666666666667</v>
       </c>
       <c r="J13">
-        <v>10845</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1009,18 +1164,18 @@
         <v>11467</v>
       </c>
       <c r="H14">
-        <v>174977.08706399999</v>
+        <v>91736.153288000001</v>
       </c>
       <c r="I14">
-        <v>867.15000000000009</v>
+        <v>480</v>
       </c>
       <c r="J14">
-        <v>12107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11467</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -1032,25 +1187,25 @@
         <v>46029</v>
       </c>
       <c r="E15">
-        <v>32175.423279999999</v>
+        <v>4879.6805999999997</v>
       </c>
       <c r="F15">
-        <v>185.41666666666666</v>
+        <v>274.58333333333337</v>
       </c>
       <c r="G15">
-        <v>10412</v>
+        <v>1066</v>
       </c>
       <c r="H15">
-        <v>109865.00522400001</v>
+        <v>12987.261269999999</v>
       </c>
       <c r="I15">
-        <v>677.15</v>
+        <v>632.85</v>
       </c>
       <c r="J15">
-        <v>9735</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1067,24 +1222,24 @@
         <v>6905.4098400000003</v>
       </c>
       <c r="F16">
-        <v>347.35</v>
+        <v>327.35000000000002</v>
       </c>
       <c r="G16">
-        <v>1193</v>
+        <v>1266</v>
       </c>
       <c r="H16">
-        <v>24536.026747</v>
+        <v>31141.082467</v>
       </c>
       <c r="I16">
-        <v>809.63333333333321</v>
+        <v>957.8</v>
       </c>
       <c r="J16">
-        <v>1818</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -1096,22 +1251,22 @@
         <v>46029</v>
       </c>
       <c r="E17">
-        <v>11785.09044</v>
+        <v>141181.84984799998</v>
       </c>
       <c r="F17">
-        <v>641.93333333333339</v>
+        <v>798.06666666666661</v>
       </c>
       <c r="G17">
-        <v>1102</v>
+        <v>10614</v>
       </c>
       <c r="H17">
-        <v>39038.469456999999</v>
+        <v>497528.17012000002</v>
       </c>
       <c r="I17">
-        <v>1575.3333333333335</v>
+        <v>2762.583333333333</v>
       </c>
       <c r="J17">
-        <v>1487</v>
+        <v>10806</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1119,7 +1274,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -1128,22 +1283,22 @@
         <v>46029</v>
       </c>
       <c r="E18">
-        <v>4879.6805999999997</v>
+        <v>11785.09044</v>
       </c>
       <c r="F18">
-        <v>294.58333333333337</v>
+        <v>601.93333333333339</v>
       </c>
       <c r="G18">
-        <v>994</v>
+        <v>1175</v>
       </c>
       <c r="H18">
-        <v>12987.261269999999</v>
+        <v>59503.564329000001</v>
       </c>
       <c r="I18">
-        <v>672.85</v>
+        <v>2277.2166666666667</v>
       </c>
       <c r="J18">
-        <v>1158</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1163,19 +1318,19 @@
         <v>57415.355640000002</v>
       </c>
       <c r="F19">
-        <v>401.83333333333331</v>
+        <v>381.83333333333331</v>
       </c>
       <c r="G19">
-        <v>8573</v>
+        <v>9022</v>
       </c>
       <c r="H19">
-        <v>78895.258031999998</v>
+        <v>227911.35256799997</v>
       </c>
       <c r="I19">
-        <v>552.20000000000005</v>
+        <v>1375.2</v>
       </c>
       <c r="J19">
-        <v>8572</v>
+        <v>9944</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1183,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -1192,27 +1347,27 @@
         <v>46030</v>
       </c>
       <c r="E20">
-        <v>135920.06883199999</v>
+        <v>78504.713191999996</v>
       </c>
       <c r="F20">
-        <v>767.13333333333333</v>
+        <v>365.3</v>
       </c>
       <c r="G20">
-        <v>10631</v>
+        <v>12894</v>
       </c>
       <c r="H20">
-        <v>442242.06351200002</v>
+        <v>284172.20400000003</v>
       </c>
       <c r="I20">
-        <v>2461.7999999999997</v>
+        <v>1345.8000000000002</v>
       </c>
       <c r="J20">
-        <v>10779</v>
+        <v>12669</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -1224,22 +1379,22 @@
         <v>46030</v>
       </c>
       <c r="E21">
-        <v>78504.713191999996</v>
+        <v>6524.1548149999999</v>
       </c>
       <c r="F21">
-        <v>365.3</v>
+        <v>114.7</v>
       </c>
       <c r="G21">
-        <v>12894</v>
+        <v>3413</v>
       </c>
       <c r="H21">
-        <v>253481.80025599999</v>
+        <v>64067.807599</v>
       </c>
       <c r="I21">
-        <v>1232.45</v>
+        <v>2243.6333333333332</v>
       </c>
       <c r="J21">
-        <v>12340</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1247,7 +1402,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1256,22 +1411,22 @@
         <v>46030</v>
       </c>
       <c r="E22">
-        <v>1865.2704000000001</v>
+        <v>20323.996009999999</v>
       </c>
       <c r="F22">
-        <v>78.166666666666657</v>
+        <v>381</v>
       </c>
       <c r="G22">
-        <v>1432</v>
+        <v>3201</v>
       </c>
       <c r="H22">
-        <v>26401.297147000001</v>
+        <v>40031.54406</v>
       </c>
       <c r="I22">
-        <v>887.79999999999984</v>
+        <v>1293.1166666666668</v>
       </c>
       <c r="J22">
-        <v>1784</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1279,7 +1434,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1288,30 +1443,30 @@
         <v>46030</v>
       </c>
       <c r="E23">
-        <v>28713.421224999998</v>
+        <v>1865.2704000000001</v>
       </c>
       <c r="F23">
-        <v>672.86666666666667</v>
+        <v>78.166666666666657</v>
       </c>
       <c r="G23">
-        <v>2560</v>
+        <v>1432</v>
       </c>
       <c r="H23">
-        <v>67751.890681999997</v>
+        <v>1865.2704000000001</v>
       </c>
       <c r="I23">
-        <v>2248.2000000000003</v>
+        <v>78.166666666666657</v>
       </c>
       <c r="J23">
-        <v>1808</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -1320,22 +1475,22 @@
         <v>46030</v>
       </c>
       <c r="E24">
-        <v>6524.1548149999999</v>
+        <v>135920.06883199999</v>
       </c>
       <c r="F24">
-        <v>114.7</v>
+        <v>747.13333333333333</v>
       </c>
       <c r="G24">
-        <v>3413</v>
+        <v>10915</v>
       </c>
       <c r="H24">
-        <v>8039.3362550000002</v>
+        <v>814123.42004</v>
       </c>
       <c r="I24">
-        <v>207.55</v>
+        <v>4220.2</v>
       </c>
       <c r="J24">
-        <v>2324</v>
+        <v>11575</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1343,7 +1498,7 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1352,22 +1507,22 @@
         <v>46030</v>
       </c>
       <c r="E25">
-        <v>20323.996009999999</v>
+        <v>28713.421224999998</v>
       </c>
       <c r="F25">
-        <v>480</v>
+        <v>573.86666666666667</v>
       </c>
       <c r="G25">
-        <v>2540</v>
+        <v>3002</v>
       </c>
       <c r="H25">
-        <v>33311.257279999998</v>
+        <v>88216.985553999999</v>
       </c>
       <c r="I25">
-        <v>1152.8499999999999</v>
+        <v>2851.0833333333335</v>
       </c>
       <c r="J25">
-        <v>1734</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1387,19 +1542,19 @@
         <v>74423.649223999993</v>
       </c>
       <c r="F26">
-        <v>480</v>
+        <v>390</v>
       </c>
       <c r="G26">
-        <v>9303</v>
+        <v>11450</v>
       </c>
       <c r="H26">
-        <v>153318.90725599998</v>
+        <v>153225.72364799998</v>
       </c>
       <c r="I26">
-        <v>1032.2</v>
+        <v>860.7166666666667</v>
       </c>
       <c r="J26">
-        <v>8912</v>
+        <v>10681</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1407,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1416,27 +1571,27 @@
         <v>46031</v>
       </c>
       <c r="E27">
-        <v>105114.052968</v>
+        <v>30690.403744000003</v>
       </c>
       <c r="F27">
-        <v>621.35</v>
+        <v>141.35</v>
       </c>
       <c r="G27">
-        <v>10150</v>
+        <v>13027</v>
       </c>
       <c r="H27">
-        <v>547356.11648000008</v>
+        <v>205667.490808</v>
       </c>
       <c r="I27">
-        <v>3083.1499999999996</v>
+        <v>980.50000000000011</v>
       </c>
       <c r="J27">
-        <v>10652</v>
+        <v>12585</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -1448,27 +1603,27 @@
         <v>46031</v>
       </c>
       <c r="E28">
-        <v>30690.403744000003</v>
+        <v>6741.8428839999997</v>
       </c>
       <c r="F28">
-        <v>141.35</v>
+        <v>288.64999999999998</v>
       </c>
       <c r="G28">
-        <v>13027</v>
+        <v>1401</v>
       </c>
       <c r="H28">
-        <v>284172.20399999997</v>
+        <v>57543.652783999998</v>
       </c>
       <c r="I28">
-        <v>1373.8</v>
+        <v>2128.9333333333334</v>
       </c>
       <c r="J28">
-        <v>12411</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -1480,22 +1635,22 @@
         <v>46031</v>
       </c>
       <c r="E29">
-        <v>6741.8428839999997</v>
+        <v>105114.052968</v>
       </c>
       <c r="F29">
-        <v>338.65</v>
+        <v>531.35</v>
       </c>
       <c r="G29">
-        <v>1194</v>
+        <v>11869</v>
       </c>
       <c r="H29">
-        <v>74493.733565999995</v>
+        <v>356346.32027200004</v>
       </c>
       <c r="I29">
-        <v>2586.8500000000004</v>
+        <v>1964.5166666666664</v>
       </c>
       <c r="J29">
-        <v>1728</v>
+        <v>10883</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1503,7 +1658,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1515,88 +1670,46 @@
         <v>6741.8428839999997</v>
       </c>
       <c r="F30">
-        <v>338.65</v>
+        <v>288.64999999999998</v>
       </c>
       <c r="G30">
-        <v>1194</v>
+        <v>1401</v>
       </c>
       <c r="H30">
-        <v>14781.179139</v>
+        <v>180583.81994400002</v>
       </c>
       <c r="I30">
-        <v>546.20000000000005</v>
+        <v>6121.2333333333327</v>
       </c>
       <c r="J30">
-        <v>1624</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
       <c r="D31" s="1">
-        <v>46034</v>
+        <v>46032</v>
       </c>
       <c r="E31">
-        <v>12276.105946</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>480</v>
-      </c>
-      <c r="G31">
-        <v>1535</v>
-      </c>
-      <c r="H31">
-        <v>38677.403093000001</v>
-      </c>
-      <c r="I31">
-        <v>1367.7999999999997</v>
-      </c>
-      <c r="J31">
-        <v>1697</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
       <c r="D32" s="1">
-        <v>46034</v>
+        <v>46033</v>
       </c>
       <c r="E32">
-        <v>12276.105946</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>480</v>
-      </c>
-      <c r="G32">
-        <v>1535</v>
-      </c>
-      <c r="H32">
-        <v>86769.839511999991</v>
-      </c>
-      <c r="I32">
-        <v>3066.8500000000004</v>
-      </c>
-      <c r="J32">
-        <v>1698</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -1605,30 +1718,30 @@
         <v>4</v>
       </c>
       <c r="D33" s="1">
-        <v>46035</v>
+        <v>46034</v>
       </c>
       <c r="E33">
-        <v>74592.445311999996</v>
+        <v>12276.105946</v>
       </c>
       <c r="F33">
-        <v>480</v>
+        <v>395</v>
       </c>
       <c r="G33">
-        <v>9324</v>
+        <v>1865</v>
       </c>
       <c r="H33">
-        <v>227911.35256799997</v>
+        <v>43417.188412999996</v>
       </c>
       <c r="I33">
-        <v>1512.2</v>
+        <v>1352.8</v>
       </c>
       <c r="J33">
-        <v>9043</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1637,25 +1750,25 @@
         <v>4</v>
       </c>
       <c r="D34" s="1">
-        <v>46035</v>
+        <v>46034</v>
       </c>
       <c r="E34">
-        <v>86092.122472000003</v>
+        <v>12276.105946</v>
       </c>
       <c r="F34">
-        <v>611.56666666666661</v>
+        <v>395</v>
       </c>
       <c r="G34">
-        <v>8446</v>
+        <v>1865</v>
       </c>
       <c r="H34">
-        <v>633448.23895200004</v>
+        <v>146880.454184</v>
       </c>
       <c r="I34">
-        <v>3694.7166666666662</v>
+        <v>4633.3166666666666</v>
       </c>
       <c r="J34">
-        <v>10287</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1681,21 +1794,21 @@
         <v>5244</v>
       </c>
       <c r="H35">
-        <v>121364.68238400001</v>
+        <v>76263.201960000006</v>
       </c>
       <c r="I35">
-        <v>808.7166666666667</v>
+        <v>501.56666666666666</v>
       </c>
       <c r="J35">
-        <v>9004</v>
+        <v>9123</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1704,22 +1817,22 @@
         <v>46035</v>
       </c>
       <c r="E36">
-        <v>14408.61191</v>
+        <v>74592.445311999996</v>
       </c>
       <c r="F36">
-        <v>828.43333333333328</v>
+        <v>453</v>
       </c>
       <c r="G36">
-        <v>1044</v>
+        <v>9880</v>
       </c>
       <c r="H36">
-        <v>101178.45142199998</v>
+        <v>78802.074423999991</v>
       </c>
       <c r="I36">
-        <v>3895.2833333333338</v>
+        <v>470.7166666666667</v>
       </c>
       <c r="J36">
-        <v>1558</v>
+        <v>10045</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1739,19 +1852,19 @@
         <v>1984.91356</v>
       </c>
       <c r="F37">
-        <v>480</v>
+        <v>31</v>
       </c>
       <c r="G37">
-        <v>248</v>
+        <v>3842</v>
       </c>
       <c r="H37">
-        <v>16766.092699000001</v>
+        <v>86227.283846999999</v>
       </c>
       <c r="I37">
-        <v>1026.2</v>
+        <v>2710.6333333333332</v>
       </c>
       <c r="J37">
-        <v>980</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1771,19 +1884,19 @@
         <v>12423.698350000001</v>
       </c>
       <c r="F38">
-        <v>348.43333333333334</v>
+        <v>268.43333333333334</v>
       </c>
       <c r="G38">
-        <v>2139</v>
+        <v>2777</v>
       </c>
       <c r="H38">
-        <v>45734.955629999997</v>
+        <v>84628.296742000006</v>
       </c>
       <c r="I38">
-        <v>1501.2833333333333</v>
+        <v>2475.8500000000004</v>
       </c>
       <c r="J38">
-        <v>1828</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1791,36 +1904,36 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="1">
-        <v>46036</v>
+        <v>46035</v>
       </c>
       <c r="E39">
-        <v>32381.7624</v>
+        <v>86092.122472000003</v>
       </c>
       <c r="F39">
-        <v>240.2</v>
+        <v>584.56666666666661</v>
       </c>
       <c r="G39">
-        <v>8089</v>
+        <v>8837</v>
       </c>
       <c r="H39">
-        <v>260293.11496799998</v>
+        <v>251232.26730400004</v>
       </c>
       <c r="I39">
-        <v>1752.4</v>
+        <v>1433.1666666666665</v>
       </c>
       <c r="J39">
-        <v>8912</v>
+        <v>10518</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
@@ -1829,25 +1942,25 @@
         <v>4</v>
       </c>
       <c r="D40" s="1">
-        <v>46036</v>
+        <v>46035</v>
       </c>
       <c r="E40">
-        <v>47032.358359999998</v>
+        <v>14408.61191</v>
       </c>
       <c r="F40">
-        <v>275.76666666666665</v>
+        <v>299.43333333333334</v>
       </c>
       <c r="G40">
-        <v>10233</v>
+        <v>2887</v>
       </c>
       <c r="H40">
-        <v>680480.597312</v>
+        <v>273990.96244600002</v>
       </c>
       <c r="I40">
-        <v>3970.4833333333327</v>
+        <v>9462.9666666666653</v>
       </c>
       <c r="J40">
-        <v>10283</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1855,7 +1968,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1864,30 +1977,30 @@
         <v>46036</v>
       </c>
       <c r="E41">
-        <v>14650.595960000001</v>
+        <v>32381.7624</v>
       </c>
       <c r="F41">
-        <v>35.566666666666663</v>
+        <v>130.19999999999999</v>
       </c>
       <c r="G41">
-        <v>24715</v>
+        <v>14922</v>
       </c>
       <c r="H41">
-        <v>298822.79995999997</v>
+        <v>260293.11496799998</v>
       </c>
       <c r="I41">
-        <v>1409.3666666666666</v>
+        <v>1505.4</v>
       </c>
       <c r="J41">
-        <v>12722</v>
+        <v>10374</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -1896,22 +2009,22 @@
         <v>46036</v>
       </c>
       <c r="E42">
-        <v>3338.2937999999999</v>
+        <v>14650.595960000001</v>
       </c>
       <c r="F42">
-        <v>90.8</v>
+        <v>35.566666666666663</v>
       </c>
       <c r="G42">
-        <v>2206</v>
+        <v>24715</v>
       </c>
       <c r="H42">
-        <v>42015.696893</v>
+        <v>298822.79996000003</v>
       </c>
       <c r="I42">
-        <v>1458.5999999999997</v>
+        <v>1381.3666666666668</v>
       </c>
       <c r="J42">
-        <v>1728</v>
+        <v>12979</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1919,7 +2032,7 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -1928,22 +2041,22 @@
         <v>46036</v>
       </c>
       <c r="E43">
-        <v>34585.193079000004</v>
+        <v>9978.9764869999999</v>
       </c>
       <c r="F43">
-        <v>1015.2333333333333</v>
+        <v>424.43333333333339</v>
       </c>
       <c r="G43">
-        <v>2044</v>
+        <v>1411</v>
       </c>
       <c r="H43">
-        <v>135763.644501</v>
+        <v>35525.568683999998</v>
       </c>
       <c r="I43">
-        <v>4910.5166666666673</v>
+        <v>1380.2833333333333</v>
       </c>
       <c r="J43">
-        <v>1659</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1951,7 +2064,7 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -1960,22 +2073,22 @@
         <v>46036</v>
       </c>
       <c r="E44">
-        <v>9978.9764869999999</v>
+        <v>21267.922792000001</v>
       </c>
       <c r="F44">
-        <v>444.43333333333339</v>
+        <v>409</v>
       </c>
       <c r="G44">
-        <v>1347</v>
+        <v>3120</v>
       </c>
       <c r="H44">
-        <v>26745.069186000001</v>
+        <v>65525.842751999997</v>
       </c>
       <c r="I44">
-        <v>1470.6333333333334</v>
+        <v>2065.9</v>
       </c>
       <c r="J44">
-        <v>1091</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1983,7 +2096,7 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -1992,22 +2105,22 @@
         <v>46036</v>
       </c>
       <c r="E45">
-        <v>21267.922792000001</v>
+        <v>3338.2937999999999</v>
       </c>
       <c r="F45">
-        <v>480</v>
+        <v>45.8</v>
       </c>
       <c r="G45">
-        <v>2658</v>
+        <v>4373</v>
       </c>
       <c r="H45">
-        <v>67002.878421999994</v>
+        <v>76643.320977999989</v>
       </c>
       <c r="I45">
-        <v>1981.2833333333333</v>
+        <v>2651.6000000000004</v>
       </c>
       <c r="J45">
-        <v>2029</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2021,57 +2134,57 @@
         <v>4</v>
       </c>
       <c r="D46" s="1">
-        <v>46037</v>
+        <v>46036</v>
       </c>
       <c r="E46">
-        <v>180675.18108800001</v>
+        <v>47032.358359999998</v>
       </c>
       <c r="F46">
-        <v>818.48333333333335</v>
+        <v>165.76666666666665</v>
       </c>
       <c r="G46">
-        <v>13245</v>
+        <v>17024</v>
       </c>
       <c r="H46">
         <v>861155.77839999995</v>
       </c>
       <c r="I46">
-        <v>4788.9666666666662</v>
+        <v>4385.9666666666662</v>
       </c>
       <c r="J46">
-        <v>10789</v>
+        <v>11781</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" s="1">
-        <v>46037</v>
+        <v>46036</v>
       </c>
       <c r="E47">
-        <v>104831.06448799999</v>
+        <v>34585.193079000004</v>
       </c>
       <c r="F47">
-        <v>480</v>
+        <v>879.23333333333335</v>
       </c>
       <c r="G47">
-        <v>13104</v>
+        <v>2360</v>
       </c>
       <c r="H47">
-        <v>403653.86444799998</v>
+        <v>134604.34823800001</v>
       </c>
       <c r="I47">
-        <v>1889.3666666666666</v>
+        <v>4238.3166666666666</v>
       </c>
       <c r="J47">
-        <v>12819</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2088,30 +2201,30 @@
         <v>46037</v>
       </c>
       <c r="E48">
-        <v>75844.116600000008</v>
+        <v>75844.116599999994</v>
       </c>
       <c r="F48">
-        <v>338.48333333333335</v>
+        <v>318.48333333333335</v>
       </c>
       <c r="G48">
-        <v>13444</v>
+        <v>14288</v>
       </c>
       <c r="H48">
-        <v>197208.79898400002</v>
+        <v>152107.31855999999</v>
       </c>
       <c r="I48">
-        <v>1147.2</v>
+        <v>820.05</v>
       </c>
       <c r="J48">
-        <v>10314</v>
+        <v>11129</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
@@ -2120,22 +2233,22 @@
         <v>46037</v>
       </c>
       <c r="E49">
-        <v>3923.1409600000002</v>
+        <v>104831.06448799999</v>
       </c>
       <c r="F49">
-        <v>331</v>
+        <v>392</v>
       </c>
       <c r="G49">
-        <v>711</v>
+        <v>16046</v>
       </c>
       <c r="H49">
-        <v>45938.837852999997</v>
+        <v>403653.86444800004</v>
       </c>
       <c r="I49">
-        <v>1789.5999999999997</v>
+        <v>1773.3666666666668</v>
       </c>
       <c r="J49">
-        <v>1540</v>
+        <v>13657</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2143,7 +2256,7 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -2152,22 +2265,22 @@
         <v>46037</v>
       </c>
       <c r="E50">
-        <v>10601.8966</v>
+        <v>6678.7556400000003</v>
       </c>
       <c r="F50">
-        <v>472.51666666666665</v>
+        <v>141.51666666666665</v>
       </c>
       <c r="G50">
-        <v>1346</v>
+        <v>2832</v>
       </c>
       <c r="H50">
-        <v>146365.54110100001</v>
+        <v>72204.598392</v>
       </c>
       <c r="I50">
-        <v>5383.0333333333338</v>
+        <v>2207.416666666667</v>
       </c>
       <c r="J50">
-        <v>1631</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2175,7 +2288,7 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -2184,54 +2297,54 @@
         <v>46037</v>
       </c>
       <c r="E51">
-        <v>6678.7556400000003</v>
+        <v>3923.1409600000002</v>
       </c>
       <c r="F51">
-        <v>141.51666666666665</v>
+        <v>266</v>
       </c>
       <c r="G51">
-        <v>2832</v>
+        <v>885</v>
       </c>
       <c r="H51">
-        <v>73681.634061999997</v>
+        <v>47340.329372999993</v>
       </c>
       <c r="I51">
-        <v>2122.8000000000002</v>
+        <v>1618.8</v>
       </c>
       <c r="J51">
-        <v>2083</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="1">
-        <v>46038</v>
+        <v>46037</v>
       </c>
       <c r="E52">
-        <v>5207.7609599999996</v>
+        <v>180675.18108799998</v>
       </c>
       <c r="F52">
-        <v>480</v>
+        <v>710.48333333333346</v>
       </c>
       <c r="G52">
-        <v>651</v>
+        <v>15258</v>
       </c>
       <c r="H52">
-        <v>51146.598812999997</v>
+        <v>678203.35120799998</v>
       </c>
       <c r="I52">
-        <v>2269.5999999999995</v>
+        <v>3473.0666666666666</v>
       </c>
       <c r="J52">
-        <v>1352</v>
+        <v>11717</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -2245,25 +2358,25 @@
         <v>4</v>
       </c>
       <c r="D53" s="1">
-        <v>46038</v>
+        <v>46037</v>
       </c>
       <c r="E53">
-        <v>29212.215083999999</v>
+        <v>10601.8966</v>
       </c>
       <c r="F53">
-        <v>1440</v>
+        <v>407.51666666666665</v>
       </c>
       <c r="G53">
-        <v>1217</v>
+        <v>1561</v>
       </c>
       <c r="H53">
-        <v>175577.75618500001</v>
+        <v>195412.09244400004</v>
       </c>
       <c r="I53">
-        <v>6823.0333333333338</v>
+        <v>6892.5333333333328</v>
       </c>
       <c r="J53">
-        <v>1544</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2283,19 +2396,19 @@
         <v>10837.454676000001</v>
       </c>
       <c r="F54">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="G54">
-        <v>1355</v>
+        <v>1414</v>
       </c>
       <c r="H54">
-        <v>37582.523862000002</v>
+        <v>130557.30383799999</v>
       </c>
       <c r="I54">
-        <v>1950.6333333333334</v>
+        <v>4228.5333333333328</v>
       </c>
       <c r="J54">
-        <v>1156</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2315,19 +2428,19 @@
         <v>13166.999448</v>
       </c>
       <c r="F55">
-        <v>479.99999999999994</v>
+        <v>459.99999999999994</v>
       </c>
       <c r="G55">
-        <v>1646</v>
+        <v>1717</v>
       </c>
       <c r="H55">
-        <v>86848.63351</v>
+        <v>97795.296190000008</v>
       </c>
       <c r="I55">
-        <v>2602.8000000000002</v>
+        <v>2935.8500000000004</v>
       </c>
       <c r="J55">
-        <v>2002</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2341,25 +2454,25 @@
         <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>46041</v>
+        <v>46038</v>
       </c>
       <c r="E56">
-        <v>5973.4565249999996</v>
+        <v>5207.7609599999996</v>
       </c>
       <c r="F56">
-        <v>72</v>
+        <v>460</v>
       </c>
       <c r="G56">
-        <v>4978</v>
+        <v>679</v>
       </c>
       <c r="H56">
-        <v>57120.055337999998</v>
+        <v>52548.090332999993</v>
       </c>
       <c r="I56">
-        <v>2341.5999999999995</v>
+        <v>2078.8000000000002</v>
       </c>
       <c r="J56">
-        <v>1464</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -2373,89 +2486,47 @@
         <v>4</v>
       </c>
       <c r="D57" s="1">
-        <v>46041</v>
+        <v>46038</v>
       </c>
       <c r="E57">
-        <v>8463.3302750000003</v>
+        <v>29212.215083999999</v>
       </c>
       <c r="F57">
-        <v>983.5</v>
+        <v>1380</v>
       </c>
       <c r="G57">
-        <v>516</v>
+        <v>1270</v>
       </c>
       <c r="H57">
-        <v>184041.08646000002</v>
+        <v>224624.30752800003</v>
       </c>
       <c r="I57">
-        <v>7806.5333333333338</v>
+        <v>8272.5333333333328</v>
       </c>
       <c r="J57">
-        <v>1415</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>8</v>
-      </c>
-      <c r="B58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s">
-        <v>4</v>
-      </c>
       <c r="D58" s="1">
-        <v>46041</v>
+        <v>46039</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>480</v>
-      </c>
-      <c r="G58">
         <v>0</v>
       </c>
-      <c r="H58">
-        <v>37582.523862000002</v>
-      </c>
-      <c r="I58">
-        <v>2430.6333333333332</v>
-      </c>
-      <c r="J58">
-        <v>928</v>
-      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>8</v>
-      </c>
-      <c r="B59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>4</v>
-      </c>
       <c r="D59" s="1">
-        <v>46041</v>
+        <v>46040</v>
       </c>
       <c r="E59">
-        <v>2489.8737500000002</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>431.5</v>
-      </c>
-      <c r="G59">
-        <v>346</v>
-      </c>
-      <c r="H59">
-        <v>89338.507259999998</v>
-      </c>
-      <c r="I59">
-        <v>3034.3</v>
-      </c>
-      <c r="J59">
-        <v>1767</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2463,31 +2534,31 @@
         <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="1">
-        <v>46042</v>
+        <v>46041</v>
       </c>
       <c r="E60">
-        <v>14783.480320000001</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="G60">
-        <v>1848</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>71903.535657999993</v>
+        <v>92160.963787000001</v>
       </c>
       <c r="I60">
-        <v>2821.5999999999995</v>
+        <v>3260.6333333333332</v>
       </c>
       <c r="J60">
-        <v>1529</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -2495,31 +2566,31 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="1">
-        <v>46042</v>
+        <v>46041</v>
       </c>
       <c r="E61">
-        <v>34958.043008000001</v>
+        <v>2489.8737500000002</v>
       </c>
       <c r="F61">
-        <v>960</v>
+        <v>171.5</v>
       </c>
       <c r="G61">
-        <v>2185</v>
+        <v>871</v>
       </c>
       <c r="H61">
-        <v>218999.12946800003</v>
+        <v>100285.16994000001</v>
       </c>
       <c r="I61">
-        <v>8766.5333333333328</v>
+        <v>3107.3500000000004</v>
       </c>
       <c r="J61">
-        <v>1499</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2527,31 +2598,31 @@
         <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="1">
-        <v>46042</v>
+        <v>46041</v>
       </c>
       <c r="E62">
-        <v>20174.562687999998</v>
+        <v>5973.4565249999996</v>
       </c>
       <c r="F62">
-        <v>480</v>
+        <v>72</v>
       </c>
       <c r="G62">
-        <v>2522</v>
+        <v>4978</v>
       </c>
       <c r="H62">
-        <v>57757.08655</v>
+        <v>73305.027177999989</v>
       </c>
       <c r="I62">
-        <v>2910.6333333333332</v>
+        <v>2605.8000000000002</v>
       </c>
       <c r="J62">
-        <v>1191</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -2565,25 +2636,25 @@
         <v>4</v>
       </c>
       <c r="D63" s="1">
-        <v>46043</v>
+        <v>46041</v>
       </c>
       <c r="E63">
-        <v>9026.7870000000003</v>
+        <v>8463.3302750000003</v>
       </c>
       <c r="F63">
-        <v>137.9</v>
+        <v>703.5</v>
       </c>
       <c r="G63">
-        <v>3928</v>
+        <v>722</v>
       </c>
       <c r="H63">
-        <v>228025.91646800004</v>
+        <v>288387.97266100004</v>
       </c>
       <c r="I63">
-        <v>8904.4333333333325</v>
+        <v>10256.466666666665</v>
       </c>
       <c r="J63">
-        <v>1536</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -2597,25 +2668,25 @@
         <v>4</v>
       </c>
       <c r="D64" s="1">
-        <v>46043</v>
+        <v>46042</v>
       </c>
       <c r="E64">
-        <v>9026.7870000000003</v>
+        <v>20174.562687999998</v>
       </c>
       <c r="F64">
-        <v>137.9</v>
+        <v>436</v>
       </c>
       <c r="G64">
-        <v>3928</v>
+        <v>2776</v>
       </c>
       <c r="H64">
-        <v>66783.873550000004</v>
+        <v>84242.370286999998</v>
       </c>
       <c r="I64">
-        <v>3048.5333333333333</v>
+        <v>2679.6333333333332</v>
       </c>
       <c r="J64">
-        <v>1314</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -2629,25 +2700,25 @@
         <v>4</v>
       </c>
       <c r="D65" s="1">
-        <v>46044</v>
+        <v>46042</v>
       </c>
       <c r="E65">
-        <v>4739.78532</v>
+        <v>14783.480320000001</v>
       </c>
       <c r="F65">
-        <v>105</v>
+        <v>455</v>
       </c>
       <c r="G65">
-        <v>2708</v>
+        <v>1949</v>
       </c>
       <c r="H65">
-        <v>76643.320977999989</v>
+        <v>67331.570652999988</v>
       </c>
       <c r="I65">
-        <v>2926.5999999999995</v>
+        <v>2533.8000000000002</v>
       </c>
       <c r="J65">
-        <v>1571</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -2661,25 +2732,25 @@
         <v>4</v>
       </c>
       <c r="D66" s="1">
-        <v>46044</v>
+        <v>46042</v>
       </c>
       <c r="E66">
-        <v>11802.169605000001</v>
+        <v>34958.043008000001</v>
       </c>
       <c r="F66">
-        <v>585</v>
+        <v>891</v>
       </c>
       <c r="G66">
-        <v>1210</v>
+        <v>2354</v>
       </c>
       <c r="H66">
-        <v>239828.08607300004</v>
+        <v>259582.35053600004</v>
       </c>
       <c r="I66">
-        <v>9489.4333333333325</v>
+        <v>9163.5333333333328</v>
       </c>
       <c r="J66">
-        <v>1516</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -2693,25 +2764,25 @@
         <v>4</v>
       </c>
       <c r="D67" s="1">
-        <v>46044</v>
+        <v>46043</v>
       </c>
       <c r="E67">
-        <v>7062.3842850000001</v>
+        <v>9026.7870000000003</v>
       </c>
       <c r="F67">
-        <v>480</v>
+        <v>137.9</v>
       </c>
       <c r="G67">
-        <v>883</v>
+        <v>3928</v>
       </c>
       <c r="H67">
-        <v>73846.257834999997</v>
+        <v>119719.849162</v>
       </c>
       <c r="I67">
-        <v>3528.5333333333333</v>
+        <v>3768.5333333333333</v>
       </c>
       <c r="J67">
-        <v>1256</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -2725,25 +2796,25 @@
         <v>4</v>
       </c>
       <c r="D68" s="1">
-        <v>46045</v>
+        <v>46043</v>
       </c>
       <c r="E68">
-        <v>18532.098375000001</v>
+        <v>9026.7870000000003</v>
       </c>
       <c r="F68">
-        <v>480</v>
+        <v>137.9</v>
       </c>
       <c r="G68">
-        <v>2317</v>
+        <v>3928</v>
       </c>
       <c r="H68">
-        <v>258360.18444800004</v>
+        <v>315946.85803600005</v>
       </c>
       <c r="I68">
-        <v>9969.4333333333325</v>
+        <v>10764.366666666665</v>
       </c>
       <c r="J68">
-        <v>1555</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -2757,89 +2828,89 @@
         <v>4</v>
       </c>
       <c r="D69" s="1">
-        <v>46045</v>
+        <v>46044</v>
       </c>
       <c r="E69">
-        <v>18532.098375000001</v>
+        <v>7062.3842850000001</v>
       </c>
       <c r="F69">
-        <v>480</v>
+        <v>403</v>
       </c>
       <c r="G69">
-        <v>2317</v>
+        <v>1051</v>
       </c>
       <c r="H69">
-        <v>92378.356209999998</v>
+        <v>24031.410756999998</v>
       </c>
       <c r="I69">
-        <v>4008.5333333333333</v>
+        <v>863</v>
       </c>
       <c r="J69">
-        <v>1383</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B70" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
       </c>
       <c r="D70" s="1">
-        <v>46048</v>
+        <v>46044</v>
       </c>
       <c r="E70">
-        <v>67338.735920000006</v>
+        <v>4739.78532</v>
       </c>
       <c r="F70">
-        <v>480</v>
+        <v>105</v>
       </c>
       <c r="G70">
-        <v>8417</v>
+        <v>2708</v>
       </c>
       <c r="H70">
-        <v>928494.51431999996</v>
+        <v>6605.0557200000003</v>
       </c>
       <c r="I70">
-        <v>5268.9666666666662</v>
+        <v>183.16666666666666</v>
       </c>
       <c r="J70">
-        <v>10573</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
       </c>
       <c r="D71" s="1">
-        <v>46048</v>
+        <v>46044</v>
       </c>
       <c r="E71">
-        <v>67338.735920000006</v>
+        <v>11802.169605000001</v>
       </c>
       <c r="F71">
-        <v>480</v>
+        <v>508</v>
       </c>
       <c r="G71">
-        <v>8417</v>
+        <v>1394</v>
       </c>
       <c r="H71">
-        <v>264547.534904</v>
+        <v>100019.155159</v>
       </c>
       <c r="I71">
-        <v>1627.2</v>
+        <v>3359.0833333333335</v>
       </c>
       <c r="J71">
-        <v>9755</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -2847,31 +2918,31 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="1">
-        <v>46048</v>
+        <v>46045</v>
       </c>
       <c r="E72">
-        <v>5933.67994</v>
+        <v>18532.098375000001</v>
       </c>
       <c r="F72">
-        <v>89.7</v>
+        <v>370</v>
       </c>
       <c r="G72">
-        <v>3969</v>
+        <v>3005</v>
       </c>
       <c r="H72">
-        <v>264293.86438800005</v>
+        <v>110693.062162</v>
       </c>
       <c r="I72">
-        <v>10059.133333333333</v>
+        <v>3630.6333333333332</v>
       </c>
       <c r="J72">
-        <v>1576</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2879,31 +2950,637 @@
         <v>8</v>
       </c>
       <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="1">
+        <v>46045</v>
+      </c>
+      <c r="E73">
+        <v>18532.098375000001</v>
+      </c>
+      <c r="F73">
+        <v>370</v>
+      </c>
+      <c r="G73">
+        <v>3005</v>
+      </c>
+      <c r="H73">
+        <v>306920.07103600004</v>
+      </c>
+      <c r="I73">
+        <v>10626.466666666665</v>
+      </c>
+      <c r="J73">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="1">
+        <v>46046</v>
+      </c>
+      <c r="E74" s="6">
+        <v>0</v>
+      </c>
+      <c r="F74" s="6">
+        <v>0</v>
+      </c>
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="1">
+        <v>46047</v>
+      </c>
+      <c r="E75" s="6">
+        <v>0</v>
+      </c>
+      <c r="F75" s="6">
+        <v>0</v>
+      </c>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="1">
+        <v>46048</v>
+      </c>
+      <c r="E76" s="6">
+        <v>67338.735920000006</v>
+      </c>
+      <c r="F76" s="6">
+        <v>388</v>
+      </c>
+      <c r="G76" s="6">
+        <v>10413</v>
+      </c>
+      <c r="H76">
+        <v>264547.534904</v>
+      </c>
+      <c r="I76">
+        <v>1495.2</v>
+      </c>
+      <c r="J76">
+        <v>10616</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C73" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="1">
+      <c r="C77" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="1">
         <v>46048</v>
       </c>
-      <c r="E73">
+      <c r="E77" s="6">
         <v>5933.67994</v>
       </c>
-      <c r="F73">
-        <v>89.7</v>
-      </c>
-      <c r="G73">
-        <v>3969</v>
-      </c>
-      <c r="H73">
-        <v>98312.03615</v>
-      </c>
-      <c r="I73">
-        <v>4098.2333333333336</v>
-      </c>
-      <c r="J73">
-        <v>1439</v>
+      <c r="F77" s="6">
+        <v>90</v>
+      </c>
+      <c r="G77" s="6">
+        <v>3956</v>
+      </c>
+      <c r="H77">
+        <v>92160.963787000001</v>
+      </c>
+      <c r="I77">
+        <v>2800.6333333333332</v>
+      </c>
+      <c r="J77">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="1">
+        <v>46048</v>
+      </c>
+      <c r="E78" s="6">
+        <v>67338.735920000006</v>
+      </c>
+      <c r="F78" s="6">
+        <v>388</v>
+      </c>
+      <c r="G78" s="6">
+        <v>10413</v>
+      </c>
+      <c r="H78">
+        <v>1073372.6788240001</v>
+      </c>
+      <c r="I78">
+        <v>5663.9666666666662</v>
+      </c>
+      <c r="J78">
+        <v>11371</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="1">
+        <v>46048</v>
+      </c>
+      <c r="E79" s="6">
+        <v>5933.67994</v>
+      </c>
+      <c r="F79" s="6">
+        <v>90</v>
+      </c>
+      <c r="G79" s="6">
+        <v>3956</v>
+      </c>
+      <c r="H79">
+        <v>279924.64238600002</v>
+      </c>
+      <c r="I79">
+        <v>9552.9666666666653</v>
+      </c>
+      <c r="J79">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="1">
+        <v>46049</v>
+      </c>
+      <c r="E80" s="6">
+        <v>33213.34016</v>
+      </c>
+      <c r="F80" s="6">
+        <v>143.11666666666667</v>
+      </c>
+      <c r="G80" s="6">
+        <v>13924</v>
+      </c>
+      <c r="H80">
+        <v>339737.648216</v>
+      </c>
+      <c r="I80">
+        <v>2078.5166666666669</v>
+      </c>
+      <c r="J80">
+        <v>9807</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="1">
+        <v>46049</v>
+      </c>
+      <c r="E81" s="6">
+        <v>16969.026471999998</v>
+      </c>
+      <c r="F81" s="6">
+        <v>460</v>
+      </c>
+      <c r="G81" s="6">
+        <v>2213</v>
+      </c>
+      <c r="H81">
+        <v>16969.026471999998</v>
+      </c>
+      <c r="I81">
+        <v>460</v>
+      </c>
+      <c r="J81">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="1">
+        <v>46049</v>
+      </c>
+      <c r="E82" s="6">
+        <v>3496.0684000000001</v>
+      </c>
+      <c r="F82" s="6">
+        <v>316.88333333333338</v>
+      </c>
+      <c r="G82" s="6">
+        <v>662</v>
+      </c>
+      <c r="H82">
+        <v>85104.384257999991</v>
+      </c>
+      <c r="I82">
+        <v>3428.4833333333336</v>
+      </c>
+      <c r="J82">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="1">
+        <v>46049</v>
+      </c>
+      <c r="E83" s="6">
+        <v>33213.34016</v>
+      </c>
+      <c r="F83" s="6">
+        <v>143.11666666666667</v>
+      </c>
+      <c r="G83" s="6">
+        <v>13924</v>
+      </c>
+      <c r="H83">
+        <v>1106586.018984</v>
+      </c>
+      <c r="I83">
+        <v>5807.083333333333</v>
+      </c>
+      <c r="J83">
+        <v>11433</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="1">
+        <v>46049</v>
+      </c>
+      <c r="E84" s="6">
+        <v>20465.094872000001</v>
+      </c>
+      <c r="F84" s="6">
+        <v>776.88333333333333</v>
+      </c>
+      <c r="G84" s="6">
+        <v>1581</v>
+      </c>
+      <c r="H84">
+        <v>20465.094872000001</v>
+      </c>
+      <c r="I84">
+        <v>776.88333333333333</v>
+      </c>
+      <c r="J84">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="1">
+        <v>46050</v>
+      </c>
+      <c r="E85" s="6">
+        <v>15276.241216</v>
+      </c>
+      <c r="F85" s="6">
+        <v>460</v>
+      </c>
+      <c r="G85" s="6">
+        <v>1993</v>
+      </c>
+      <c r="H85">
+        <v>50801.8099</v>
+      </c>
+      <c r="I85">
+        <v>1840.2833333333333</v>
+      </c>
+      <c r="J85">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="1">
+        <v>46050</v>
+      </c>
+      <c r="E86" s="6">
+        <v>6720.2867800000004</v>
+      </c>
+      <c r="F86" s="6">
+        <v>279.26666666666665</v>
+      </c>
+      <c r="G86" s="6">
+        <v>1444</v>
+      </c>
+      <c r="H86">
+        <v>19707.548049999998</v>
+      </c>
+      <c r="I86">
+        <v>912.11666666666667</v>
+      </c>
+      <c r="J86">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="1">
+        <v>46050</v>
+      </c>
+      <c r="E87" s="6">
+        <v>4964.9948800000002</v>
+      </c>
+      <c r="F87" s="6">
+        <v>460</v>
+      </c>
+      <c r="G87" s="6">
+        <v>648</v>
+      </c>
+      <c r="H87">
+        <v>81608.315857999987</v>
+      </c>
+      <c r="I87">
+        <v>3111.6000000000004</v>
+      </c>
+      <c r="J87">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="1">
+        <v>46050</v>
+      </c>
+      <c r="E88" s="6">
+        <v>26961.522875999999</v>
+      </c>
+      <c r="F88" s="6">
+        <v>1199.2666666666664</v>
+      </c>
+      <c r="G88" s="6">
+        <v>1349</v>
+      </c>
+      <c r="H88">
+        <v>173841.97706</v>
+      </c>
+      <c r="I88">
+        <v>5832.583333333333</v>
+      </c>
+      <c r="J88">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="1">
+        <v>46051</v>
+      </c>
+      <c r="E89" s="6">
+        <v>46231.193088</v>
+      </c>
+      <c r="F89" s="6">
+        <v>430</v>
+      </c>
+      <c r="G89" s="6">
+        <v>6451</v>
+      </c>
+      <c r="H89">
+        <v>306524.30805599998</v>
+      </c>
+      <c r="I89">
+        <v>1935.4</v>
+      </c>
+      <c r="J89">
+        <v>9503</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="1">
+        <v>46051</v>
+      </c>
+      <c r="E90" s="6">
+        <v>98646.971416000015</v>
+      </c>
+      <c r="F90" s="6">
+        <v>460</v>
+      </c>
+      <c r="G90" s="6">
+        <v>12867</v>
+      </c>
+      <c r="H90">
+        <v>502300.83586400002</v>
+      </c>
+      <c r="I90">
+        <v>2233.3666666666668</v>
+      </c>
+      <c r="J90">
+        <v>13494</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="1">
+        <v>46051</v>
+      </c>
+      <c r="E91" s="6">
+        <v>4226.3759</v>
+      </c>
+      <c r="F91" s="6">
+        <v>363.78333333333336</v>
+      </c>
+      <c r="G91" s="6">
+        <v>697</v>
+      </c>
+      <c r="H91">
+        <v>44257.919959999999</v>
+      </c>
+      <c r="I91">
+        <v>1656.9</v>
+      </c>
+      <c r="J91">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="1">
+        <v>46051</v>
+      </c>
+      <c r="E92" s="6">
+        <v>144878.16450400001</v>
+      </c>
+      <c r="F92" s="6">
+        <v>890</v>
+      </c>
+      <c r="G92" s="6">
+        <v>9767</v>
+      </c>
+      <c r="H92">
+        <v>1006033.9429039999</v>
+      </c>
+      <c r="I92">
+        <v>5275.9666666666662</v>
+      </c>
+      <c r="J92">
+        <v>11441</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="1">
+        <v>46051</v>
+      </c>
+      <c r="E93" s="6">
+        <v>4226.3759</v>
+      </c>
+      <c r="F93" s="6">
+        <v>363.78333333333336</v>
+      </c>
+      <c r="G93" s="6">
+        <v>697</v>
+      </c>
+      <c r="H93">
+        <v>184810.19584400003</v>
+      </c>
+      <c r="I93">
+        <v>6485.0166666666664</v>
+      </c>
+      <c r="J93">
+        <v>1710</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update performance chart to use day index for sliding window
Modify the API to include `day_index` for each unique date, and update the frontend JavaScript to utilize this `day_index` for the sliding window mechanism on the performance chart, ensuring data is filtered based on this technical column.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ab82b662-954a-45ad-9e37-a64a43e3529b
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 5b7221bf-1026-4807-adc6-cc5a8f1cbf70
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d7b551d1-b37d-40c2-8d39-61fe8a04a1c4/ab82b662-954a-45ad-9e37-a64a43e3529b/ZT1Iu2n
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/Jumbo.xlsx
+++ b/Jumbo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://storaenso-my.sharepoint.com/personal/dariusz_buchalski_storaenso_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{2C740303-9498-4E1B-B999-D732A592522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CF4CF80-B2B3-4F3C-85B9-6E277A944BB0}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{2C740303-9498-4E1B-B999-D732A592522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31DF8235-8E6D-4EAF-9734-089E9661F991}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE0CCD2D-10B9-4F52-863F-7EF4C64C1846}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="28">
   <si>
     <t>Segment</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Python</t>
+  </si>
+  <si>
+    <t>day_index</t>
   </si>
 </sst>
 </file>
@@ -234,19 +237,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -283,8 +288,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_3" connectionId="1" xr16:uid="{190A9E09-10C5-4272-AEC7-483C4BD0B906}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="22">
-    <queryTableFields count="10">
+  <queryTableRefresh nextId="23" unboundColumnsRight="1">
+    <queryTableFields count="11">
       <queryTableField id="2" name="Segment" tableColumnId="2"/>
       <queryTableField id="3" name="Brygada" tableColumnId="3"/>
       <queryTableField id="14" name="mtf_costcenter_number" tableColumnId="11"/>
@@ -295,28 +300,32 @@
       <queryTableField id="16" name="Cum_Prod_m2" tableColumnId="6"/>
       <queryTableField id="17" name="Cum_WorkMin" tableColumnId="7"/>
       <queryTableField id="18" name="Cum_Speed_m2_wh" tableColumnId="8"/>
+      <queryTableField id="22" dataBound="0" tableColumnId="9"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}" name="Raport" displayName="Raport" ref="A1:J93" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:J93" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}" name="Raport" displayName="Raport" ref="A1:K93" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:K93" xr:uid="{1730138A-E642-433B-AAA9-F2A57BDF5BDE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J73">
     <sortCondition ref="D2:D73"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{A434A7BD-B920-46DC-B679-B95F31C0C848}" uniqueName="2" name="Segment" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C0E9884D-F486-48B7-87A5-4F055B5CB66D}" uniqueName="3" name="Brygada" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{F9452BD7-48CB-4743-BE47-B2D814028231}" uniqueName="11" name="Maszyna" queryTableFieldId="14" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{41D9B31B-1C8D-4046-97C1-641A0512F4FF}" uniqueName="1" name="Dzień" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1BE80ADB-A0F6-4E35-9F75-8589EBAC253C}" uniqueName="4" name="Produkcja dzienna [m2 ]" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{8ADC085E-8895-4FE1-B278-28AC47A635AF}" uniqueName="5" name="Czas pracy [wh]" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{F0074E8F-F181-49E0-AA94-E5179D277904}" uniqueName="10" name="Prędkość dzienna [m2/wh]" queryTableFieldId="13" dataDxfId="0"/>
+  <tableColumns count="11">
+    <tableColumn id="2" xr3:uid="{A434A7BD-B920-46DC-B679-B95F31C0C848}" uniqueName="2" name="Segment" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C0E9884D-F486-48B7-87A5-4F055B5CB66D}" uniqueName="3" name="Brygada" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{F9452BD7-48CB-4743-BE47-B2D814028231}" uniqueName="11" name="Maszyna" queryTableFieldId="14" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{41D9B31B-1C8D-4046-97C1-641A0512F4FF}" uniqueName="1" name="Dzień" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1BE80ADB-A0F6-4E35-9F75-8589EBAC253C}" uniqueName="4" name="Produkcja dzienna [m2 ]" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8ADC085E-8895-4FE1-B278-28AC47A635AF}" uniqueName="5" name="Czas pracy [wh]" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{F0074E8F-F181-49E0-AA94-E5179D277904}" uniqueName="10" name="Prędkość dzienna [m2/wh]" queryTableFieldId="13" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{0851AB8C-C656-465B-A3A0-36796443A497}" uniqueName="6" name="Narastająca produkcja [m2]" queryTableFieldId="16"/>
     <tableColumn id="7" xr3:uid="{F2C67B8B-BAF4-4581-B1A3-A0321B5720DA}" uniqueName="7" name="Narastający czas [wh]" queryTableFieldId="17"/>
     <tableColumn id="8" xr3:uid="{F02E25EB-ABDC-4BEA-A110-810B00100C01}" uniqueName="8" name="Narastająca prędkość [m2/wh]" queryTableFieldId="18"/>
+    <tableColumn id="9" xr3:uid="{601B24B1-0C4F-4661-AE6D-C73DBFC7663A}" uniqueName="9" name="day_index" queryTableFieldId="22" dataDxfId="0">
+      <calculatedColumnFormula>DAY(Raport[[#This Row],[Dzień]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -641,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309D4C89-61CE-4AA4-A671-398E4FB3D027}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +664,7 @@
     <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
     <col min="13" max="13" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.42578125" customWidth="1"/>
   </cols>
@@ -690,6 +700,9 @@
       <c r="J1" t="s">
         <v>11</v>
       </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -722,6 +735,10 @@
       <c r="J2">
         <v>10502</v>
       </c>
+      <c r="K2">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>5</v>
+      </c>
       <c r="M2" t="s">
         <v>26</v>
       </c>
@@ -760,6 +777,10 @@
       <c r="J3">
         <v>10502</v>
       </c>
+      <c r="K3">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>5</v>
+      </c>
       <c r="M3" s="2" t="s">
         <v>0</v>
       </c>
@@ -798,6 +819,10 @@
       <c r="J4">
         <v>10742</v>
       </c>
+      <c r="K4">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
+      </c>
       <c r="M4" s="3" t="s">
         <v>1</v>
       </c>
@@ -836,6 +861,10 @@
       <c r="J5">
         <v>14257</v>
       </c>
+      <c r="K5">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
+      </c>
       <c r="M5" s="3" t="s">
         <v>9</v>
       </c>
@@ -874,6 +903,10 @@
       <c r="J6">
         <v>12511</v>
       </c>
+      <c r="K6">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
+      </c>
       <c r="M6" s="5" t="s">
         <v>10</v>
       </c>
@@ -912,6 +945,10 @@
       <c r="J7">
         <v>1604</v>
       </c>
+      <c r="K7">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
+      </c>
       <c r="M7" s="3" t="s">
         <v>15</v>
       </c>
@@ -950,6 +987,10 @@
       <c r="J8">
         <v>1358</v>
       </c>
+      <c r="K8">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
+      </c>
       <c r="M8" s="3" t="s">
         <v>14</v>
       </c>
@@ -987,6 +1028,10 @@
       </c>
       <c r="J9">
         <v>2307</v>
+      </c>
+      <c r="K9">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>13</v>
@@ -1026,6 +1071,10 @@
       <c r="J10">
         <v>11676</v>
       </c>
+      <c r="K10">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
+      </c>
       <c r="M10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1063,6 +1112,10 @@
       </c>
       <c r="J11">
         <v>1709</v>
+      </c>
+      <c r="K11">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>6</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>16</v>
@@ -1102,6 +1155,10 @@
       <c r="J12">
         <v>10687</v>
       </c>
+      <c r="K12">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>7</v>
+      </c>
       <c r="M12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1140,6 +1197,10 @@
       <c r="J13">
         <v>10298</v>
       </c>
+      <c r="K13">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1172,6 +1233,10 @@
       <c r="J14">
         <v>11467</v>
       </c>
+      <c r="K14">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1204,6 +1269,10 @@
       <c r="J15">
         <v>1231</v>
       </c>
+      <c r="K15">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1236,8 +1305,12 @@
       <c r="J16">
         <v>1951</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1268,8 +1341,12 @@
       <c r="J17">
         <v>10806</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1300,8 +1377,12 @@
       <c r="J18">
         <v>1568</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1332,8 +1413,12 @@
       <c r="J19">
         <v>9944</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1364,8 +1449,12 @@
       <c r="J20">
         <v>12669</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1396,8 +1485,12 @@
       <c r="J21">
         <v>1713</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1428,8 +1521,12 @@
       <c r="J22">
         <v>1857</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1460,8 +1557,12 @@
       <c r="J23">
         <v>1432</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1492,8 +1593,12 @@
       <c r="J24">
         <v>11575</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1524,8 +1629,12 @@
       <c r="J25">
         <v>1856</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1556,8 +1665,12 @@
       <c r="J26">
         <v>10681</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1588,8 +1701,12 @@
       <c r="J27">
         <v>12585</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1620,8 +1737,12 @@
       <c r="J28">
         <v>1622</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1652,8 +1773,12 @@
       <c r="J29">
         <v>10883</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1684,8 +1809,12 @@
       <c r="J30">
         <v>1770</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <v>46032</v>
       </c>
@@ -1695,8 +1824,12 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <v>46033</v>
       </c>
@@ -1706,8 +1839,12 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1738,8 +1875,12 @@
       <c r="J33">
         <v>1926</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1770,8 +1911,12 @@
       <c r="J34">
         <v>1902</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1802,8 +1947,12 @@
       <c r="J35">
         <v>9123</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -1834,8 +1983,12 @@
       <c r="J36">
         <v>10045</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1866,8 +2019,12 @@
       <c r="J37">
         <v>1909</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1898,8 +2055,12 @@
       <c r="J38">
         <v>2051</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1930,8 +2091,12 @@
       <c r="J39">
         <v>10518</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1962,8 +2127,12 @@
       <c r="J40">
         <v>1737</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -1994,8 +2163,12 @@
       <c r="J41">
         <v>10374</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2026,8 +2199,12 @@
       <c r="J42">
         <v>12979</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2058,8 +2235,12 @@
       <c r="J43">
         <v>1544</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2090,8 +2271,12 @@
       <c r="J44">
         <v>1903</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2122,8 +2307,12 @@
       <c r="J45">
         <v>1734</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -2154,8 +2343,12 @@
       <c r="J46">
         <v>11781</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2186,8 +2379,12 @@
       <c r="J47">
         <v>1906</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -2218,8 +2415,12 @@
       <c r="J48">
         <v>11129</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2250,8 +2451,12 @@
       <c r="J49">
         <v>13657</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2282,8 +2487,12 @@
       <c r="J50">
         <v>1963</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2314,8 +2523,12 @@
       <c r="J51">
         <v>1755</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -2346,8 +2559,12 @@
       <c r="J52">
         <v>11717</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2378,8 +2595,12 @@
       <c r="J53">
         <v>1701</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2410,8 +2631,12 @@
       <c r="J54">
         <v>1853</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2442,8 +2667,12 @@
       <c r="J55">
         <v>1999</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2474,8 +2703,12 @@
       <c r="J56">
         <v>1517</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2506,8 +2739,12 @@
       <c r="J57">
         <v>1629</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D58" s="1">
         <v>46039</v>
       </c>
@@ -2517,8 +2754,12 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D59" s="1">
         <v>46040</v>
       </c>
@@ -2528,8 +2769,12 @@
       <c r="F59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -2560,8 +2805,12 @@
       <c r="J60">
         <v>1696</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -2592,8 +2841,12 @@
       <c r="J61">
         <v>1936</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -2624,8 +2877,12 @@
       <c r="J62">
         <v>1688</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -2656,8 +2913,12 @@
       <c r="J63">
         <v>1687</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -2688,8 +2949,12 @@
       <c r="J64">
         <v>1886</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2720,8 +2985,12 @@
       <c r="J65">
         <v>1594</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2752,8 +3021,12 @@
       <c r="J66">
         <v>1700</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -2784,8 +3057,12 @@
       <c r="J67">
         <v>1906</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -2816,8 +3093,12 @@
       <c r="J68">
         <v>1761</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -2848,8 +3129,12 @@
       <c r="J69">
         <v>1671</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -2880,8 +3165,12 @@
       <c r="J70">
         <v>2164</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -2912,8 +3201,12 @@
       <c r="J71">
         <v>1787</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -2944,8 +3237,12 @@
       <c r="J72">
         <v>1829</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2976,57 +3273,61 @@
       <c r="J73">
         <v>1733</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
+      <c r="K73">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D74" s="1">
         <v>46046</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E74">
         <v>0</v>
       </c>
-      <c r="F74" s="6">
+      <c r="F74">
         <v>0</v>
       </c>
-      <c r="G74" s="6"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
+      <c r="K74">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D75" s="1">
         <v>46047</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E75">
         <v>0</v>
       </c>
-      <c r="F75" s="6">
+      <c r="F75">
         <v>0</v>
       </c>
-      <c r="G75" s="6"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
+      <c r="K75">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C76" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="1">
         <v>46048</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76">
         <v>67338.735920000006</v>
       </c>
-      <c r="F76" s="6">
+      <c r="F76">
         <v>388</v>
       </c>
-      <c r="G76" s="6">
+      <c r="G76">
         <v>10413</v>
       </c>
       <c r="H76">
@@ -3038,27 +3339,31 @@
       <c r="J76">
         <v>10616</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" s="6" t="s">
+      <c r="K76">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" t="s">
         <v>7</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" t="s">
         <v>4</v>
       </c>
       <c r="D77" s="1">
         <v>46048</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E77">
         <v>5933.67994</v>
       </c>
-      <c r="F77" s="6">
+      <c r="F77">
         <v>90</v>
       </c>
-      <c r="G77" s="6">
+      <c r="G77">
         <v>3956</v>
       </c>
       <c r="H77">
@@ -3070,27 +3375,31 @@
       <c r="J77">
         <v>1974</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
+      <c r="K77">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>2</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" t="s">
         <v>4</v>
       </c>
       <c r="D78" s="1">
         <v>46048</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78">
         <v>67338.735920000006</v>
       </c>
-      <c r="F78" s="6">
+      <c r="F78">
         <v>388</v>
       </c>
-      <c r="G78" s="6">
+      <c r="G78">
         <v>10413</v>
       </c>
       <c r="H78">
@@ -3102,27 +3411,31 @@
       <c r="J78">
         <v>11371</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B79" s="6" t="s">
+      <c r="K78">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
         <v>3</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" t="s">
         <v>4</v>
       </c>
       <c r="D79" s="1">
         <v>46048</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79">
         <v>5933.67994</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F79">
         <v>90</v>
       </c>
-      <c r="G79" s="6">
+      <c r="G79">
         <v>3956</v>
       </c>
       <c r="H79">
@@ -3134,27 +3447,31 @@
       <c r="J79">
         <v>1758</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+      <c r="K79">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="1">
         <v>46049</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80">
         <v>33213.34016</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F80">
         <v>143.11666666666667</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G80">
         <v>13924</v>
       </c>
       <c r="H80">
@@ -3166,27 +3483,31 @@
       <c r="J80">
         <v>9807</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B81" s="6" t="s">
+      <c r="K80">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>8</v>
+      </c>
+      <c r="B81" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" t="s">
         <v>4</v>
       </c>
       <c r="D81" s="1">
         <v>46049</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81">
         <v>16969.026471999998</v>
       </c>
-      <c r="F81" s="6">
+      <c r="F81">
         <v>460</v>
       </c>
-      <c r="G81" s="6">
+      <c r="G81">
         <v>2213</v>
       </c>
       <c r="H81">
@@ -3198,27 +3519,31 @@
       <c r="J81">
         <v>2213</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="6" t="s">
+      <c r="K81">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="1">
         <v>46049</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82">
         <v>3496.0684000000001</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F82">
         <v>316.88333333333338</v>
       </c>
-      <c r="G82" s="6">
+      <c r="G82">
         <v>662</v>
       </c>
       <c r="H82">
@@ -3230,27 +3555,31 @@
       <c r="J82">
         <v>1489</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
+      <c r="K82">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>2</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" t="s">
         <v>3</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" t="s">
         <v>4</v>
       </c>
       <c r="D83" s="1">
         <v>46049</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83">
         <v>33213.34016</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83">
         <v>143.11666666666667</v>
       </c>
-      <c r="G83" s="6">
+      <c r="G83">
         <v>13924</v>
       </c>
       <c r="H83">
@@ -3262,27 +3591,31 @@
       <c r="J83">
         <v>11433</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B84" s="6" t="s">
+      <c r="K83">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="1">
         <v>46049</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84">
         <v>20465.094872000001</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F84">
         <v>776.88333333333333</v>
       </c>
-      <c r="G84" s="6">
+      <c r="G84">
         <v>1581</v>
       </c>
       <c r="H84">
@@ -3294,27 +3627,31 @@
       <c r="J84">
         <v>1581</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B85" s="6" t="s">
+      <c r="K84">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" t="s">
         <v>4</v>
       </c>
       <c r="D85" s="1">
         <v>46050</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E85">
         <v>15276.241216</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F85">
         <v>460</v>
       </c>
-      <c r="G85" s="6">
+      <c r="G85">
         <v>1993</v>
       </c>
       <c r="H85">
@@ -3326,27 +3663,31 @@
       <c r="J85">
         <v>1656</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B86" s="6" t="s">
+      <c r="K85">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" t="s">
         <v>4</v>
       </c>
       <c r="D86" s="1">
         <v>46050</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E86">
         <v>6720.2867800000004</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F86">
         <v>279.26666666666665</v>
       </c>
-      <c r="G86" s="6">
+      <c r="G86">
         <v>1444</v>
       </c>
       <c r="H86">
@@ -3358,27 +3699,31 @@
       <c r="J86">
         <v>1296</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B87" s="6" t="s">
+      <c r="K86">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" t="s">
         <v>6</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" t="s">
         <v>4</v>
       </c>
       <c r="D87" s="1">
         <v>46050</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E87">
         <v>4964.9948800000002</v>
       </c>
-      <c r="F87" s="6">
+      <c r="F87">
         <v>460</v>
       </c>
-      <c r="G87" s="6">
+      <c r="G87">
         <v>648</v>
       </c>
       <c r="H87">
@@ -3390,27 +3735,31 @@
       <c r="J87">
         <v>1574</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B88" s="6" t="s">
+      <c r="K87">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" t="s">
         <v>3</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="1">
         <v>46050</v>
       </c>
-      <c r="E88" s="6">
+      <c r="E88">
         <v>26961.522875999999</v>
       </c>
-      <c r="F88" s="6">
+      <c r="F88">
         <v>1199.2666666666664</v>
       </c>
-      <c r="G88" s="6">
+      <c r="G88">
         <v>1349</v>
       </c>
       <c r="H88">
@@ -3422,27 +3771,31 @@
       <c r="J88">
         <v>1788</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+      <c r="K88">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>2</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" t="s">
         <v>4</v>
       </c>
       <c r="D89" s="1">
         <v>46051</v>
       </c>
-      <c r="E89" s="6">
+      <c r="E89">
         <v>46231.193088</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F89">
         <v>430</v>
       </c>
-      <c r="G89" s="6">
+      <c r="G89">
         <v>6451</v>
       </c>
       <c r="H89">
@@ -3454,27 +3807,31 @@
       <c r="J89">
         <v>9503</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
+      <c r="K89">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>2</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" t="s">
         <v>7</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" t="s">
         <v>4</v>
       </c>
       <c r="D90" s="1">
         <v>46051</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E90">
         <v>98646.971416000015</v>
       </c>
-      <c r="F90" s="6">
+      <c r="F90">
         <v>460</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G90">
         <v>12867</v>
       </c>
       <c r="H90">
@@ -3486,27 +3843,31 @@
       <c r="J90">
         <v>13494</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B91" s="6" t="s">
+      <c r="K90">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" t="s">
         <v>4</v>
       </c>
       <c r="D91" s="1">
         <v>46051</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E91">
         <v>4226.3759</v>
       </c>
-      <c r="F91" s="6">
+      <c r="F91">
         <v>363.78333333333336</v>
       </c>
-      <c r="G91" s="6">
+      <c r="G91">
         <v>697</v>
       </c>
       <c r="H91">
@@ -3518,27 +3879,31 @@
       <c r="J91">
         <v>1603</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="K91">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>2</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" t="s">
         <v>3</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C92" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="1">
         <v>46051</v>
       </c>
-      <c r="E92" s="6">
+      <c r="E92">
         <v>144878.16450400001</v>
       </c>
-      <c r="F92" s="6">
+      <c r="F92">
         <v>890</v>
       </c>
-      <c r="G92" s="6">
+      <c r="G92">
         <v>9767</v>
       </c>
       <c r="H92">
@@ -3550,27 +3915,31 @@
       <c r="J92">
         <v>11441</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B93" s="6" t="s">
+      <c r="K92">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C93" t="s">
         <v>4</v>
       </c>
       <c r="D93" s="1">
         <v>46051</v>
       </c>
-      <c r="E93" s="6">
+      <c r="E93">
         <v>4226.3759</v>
       </c>
-      <c r="F93" s="6">
+      <c r="F93">
         <v>363.78333333333336</v>
       </c>
-      <c r="G93" s="6">
+      <c r="G93">
         <v>697</v>
       </c>
       <c r="H93">
@@ -3581,6 +3950,10 @@
       </c>
       <c r="J93">
         <v>1710</v>
+      </c>
+      <c r="K93">
+        <f>DAY(Raport[[#This Row],[Dzień]])</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>